<commit_message>
Se arregló el diseño de la vista Lector de Excel y también de la vista Datos
</commit_message>
<xml_diff>
--- a/Tarea4/Lector/Prueba.xlsx
+++ b/Tarea4/Lector/Prueba.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Nombre</t>
   </si>
@@ -49,6 +49,21 @@
   </si>
   <si>
     <t xml:space="preserve">Guerrero </t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Yuleisi</t>
+  </si>
+  <si>
+    <t>Feliz</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Villaman</t>
   </si>
 </sst>
 </file>
@@ -366,15 +381,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,8 +402,11 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -401,8 +419,11 @@
       <c r="D2">
         <v>20186304</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -415,8 +436,11 @@
       <c r="D3">
         <v>20186299</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -428,6 +452,43 @@
       </c>
       <c r="D4">
         <v>20186603</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>20184432</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>52</v>
+      </c>
+      <c r="D6">
+        <v>20184321</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se arregló la lógica del lector de Excel
</commit_message>
<xml_diff>
--- a/Tarea4/Lector/Prueba.xlsx
+++ b/Tarea4/Lector/Prueba.xlsx
@@ -19,51 +19,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Apellido</t>
-  </si>
-  <si>
-    <t>Edad</t>
-  </si>
-  <si>
-    <t>Erlyn</t>
-  </si>
-  <si>
-    <t>Taveras</t>
-  </si>
-  <si>
-    <t>Matrícula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jesús </t>
-  </si>
-  <si>
-    <t>Estévez</t>
-  </si>
-  <si>
-    <t>Wilmer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guerrero </t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Yuleisi</t>
-  </si>
-  <si>
-    <t>Feliz</t>
-  </si>
-  <si>
-    <t>Mary</t>
-  </si>
-  <si>
-    <t>Villaman</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="12">
+  <si>
+    <t>Col2</t>
+  </si>
+  <si>
+    <t>Col3</t>
+  </si>
+  <si>
+    <t>Col4</t>
+  </si>
+  <si>
+    <t>Col5</t>
+  </si>
+  <si>
+    <t>Row1</t>
+  </si>
+  <si>
+    <t>Row2</t>
+  </si>
+  <si>
+    <t>Row3</t>
+  </si>
+  <si>
+    <t>Row4</t>
+  </si>
+  <si>
+    <t>Row5</t>
+  </si>
+  <si>
+    <t>Row6</t>
+  </si>
+  <si>
+    <t>Row7</t>
+  </si>
+  <si>
+    <t>Col1</t>
   </si>
 </sst>
 </file>
@@ -99,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,117 +373,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>20186304</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>20</v>
-      </c>
-      <c r="D3">
-        <v>20186299</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>19</v>
-      </c>
-      <c r="D4">
-        <v>20186603</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>18</v>
-      </c>
-      <c r="D5">
-        <v>20184432</v>
-      </c>
-      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>52</v>
-      </c>
-      <c r="D6">
-        <v>20184321</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>